<commit_message>
feat: add id on excel
</commit_message>
<xml_diff>
--- a/app/static/sheet1.xlsx
+++ b/app/static/sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dada/workspace/fix_grid/app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92535CEE-7968-334F-A496-9F910F19CF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F806AD7B-53E4-E34A-ABD2-35204C1B0F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="16760" tabRatio="897" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -908,6 +908,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -936,12 +942,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1275,8 +1275,8 @@
   <dimension ref="A1:U74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="4" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -1300,62 +1300,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="31.5" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="I1" s="38" t="s">
+      <c r="B1" s="38"/>
+      <c r="I1" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
     </row>
     <row r="2" spans="1:21" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="1:21" ht="34.5" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="43" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="45"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="47"/>
     </row>
     <row r="4" spans="1:21" ht="50.25" customHeight="1">
       <c r="A4" s="22" t="s">
@@ -1385,7 +1385,7 @@
       <c r="I4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="36" t="s">
         <v>33</v>
       </c>
       <c r="K4" s="29" t="s">
@@ -1408,9 +1408,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A5" s="11">
-        <v>1</v>
-      </c>
+      <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1428,9 +1426,7 @@
       <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A6" s="11">
-        <v>2</v>
-      </c>
+      <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
@@ -1451,9 +1447,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A7" s="11">
-        <v>3</v>
-      </c>
+      <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
@@ -1474,9 +1468,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A8" s="11">
-        <v>4</v>
-      </c>
+      <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
@@ -1494,9 +1486,7 @@
       <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A9" s="11">
-        <v>5</v>
-      </c>
+      <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
@@ -1514,9 +1504,7 @@
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A10" s="30">
-        <v>6</v>
-      </c>
+      <c r="A10" s="30"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
@@ -1534,9 +1522,7 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A11" s="11">
-        <v>7</v>
-      </c>
+      <c r="A11" s="11"/>
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
       <c r="D11" s="33"/>
@@ -1545,7 +1531,7 @@
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="47"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="34"/>
       <c r="L11" s="31"/>
       <c r="M11" s="12"/>
@@ -1554,9 +1540,7 @@
       <c r="P11" s="14"/>
     </row>
     <row r="12" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A12" s="11">
-        <v>8</v>
-      </c>
+      <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -1574,9 +1558,7 @@
       <c r="P12" s="14"/>
     </row>
     <row r="13" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A13" s="11">
-        <v>9</v>
-      </c>
+      <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
@@ -1594,9 +1576,7 @@
       <c r="P13" s="14"/>
     </row>
     <row r="14" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A14" s="11">
-        <v>10</v>
-      </c>
+      <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
@@ -1614,9 +1594,7 @@
       <c r="P14" s="14"/>
     </row>
     <row r="15" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A15" s="11">
-        <v>11</v>
-      </c>
+      <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1634,9 +1612,7 @@
       <c r="P15" s="14"/>
     </row>
     <row r="16" spans="1:21" ht="39.75" customHeight="1">
-      <c r="A16" s="11">
-        <v>12</v>
-      </c>
+      <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1654,9 +1630,7 @@
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A17" s="11">
-        <v>13</v>
-      </c>
+      <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
@@ -1674,9 +1648,7 @@
       <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A18" s="11">
-        <v>14</v>
-      </c>
+      <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
@@ -1694,9 +1666,7 @@
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A19" s="11">
-        <v>15</v>
-      </c>
+      <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>
@@ -1714,9 +1684,7 @@
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A20" s="11">
-        <v>16</v>
-      </c>
+      <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
@@ -1734,9 +1702,7 @@
       <c r="P20" s="14"/>
     </row>
     <row r="21" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A21" s="11">
-        <v>17</v>
-      </c>
+      <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="13"/>
@@ -1754,9 +1720,7 @@
       <c r="P21" s="14"/>
     </row>
     <row r="22" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A22" s="11">
-        <v>18</v>
-      </c>
+      <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -1774,9 +1738,7 @@
       <c r="P22" s="14"/>
     </row>
     <row r="23" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A23" s="11">
-        <v>19</v>
-      </c>
+      <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
@@ -1794,9 +1756,7 @@
       <c r="P23" s="14"/>
     </row>
     <row r="24" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A24" s="11">
-        <v>20</v>
-      </c>
+      <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
@@ -1814,9 +1774,7 @@
       <c r="P24" s="14"/>
     </row>
     <row r="25" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A25" s="11">
-        <v>21</v>
-      </c>
+      <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
@@ -1834,9 +1792,7 @@
       <c r="P25" s="14"/>
     </row>
     <row r="26" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A26" s="11">
-        <v>22</v>
-      </c>
+      <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
@@ -1854,9 +1810,7 @@
       <c r="P26" s="14"/>
     </row>
     <row r="27" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A27" s="11">
-        <v>23</v>
-      </c>
+      <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13"/>
@@ -1874,9 +1828,7 @@
       <c r="P27" s="14"/>
     </row>
     <row r="28" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A28" s="11">
-        <v>24</v>
-      </c>
+      <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
@@ -1894,9 +1846,7 @@
       <c r="P28" s="14"/>
     </row>
     <row r="29" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A29" s="11">
-        <v>25</v>
-      </c>
+      <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="13"/>
@@ -1914,9 +1864,7 @@
       <c r="P29" s="14"/>
     </row>
     <row r="30" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A30" s="11">
-        <v>26</v>
-      </c>
+      <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
@@ -1934,9 +1882,7 @@
       <c r="P30" s="14"/>
     </row>
     <row r="31" spans="1:16" s="5" customFormat="1" ht="138" customHeight="1">
-      <c r="A31" s="11">
-        <v>27</v>
-      </c>
+      <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="13"/>
@@ -1954,9 +1900,7 @@
       <c r="P31" s="14"/>
     </row>
     <row r="32" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A32" s="11">
-        <v>28</v>
-      </c>
+      <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
@@ -1974,9 +1918,7 @@
       <c r="P32" s="14"/>
     </row>
     <row r="33" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A33" s="11">
-        <v>29</v>
-      </c>
+      <c r="A33" s="11"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="13"/>
@@ -1994,9 +1936,7 @@
       <c r="P33" s="14"/>
     </row>
     <row r="34" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A34" s="11">
-        <v>30</v>
-      </c>
+      <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
@@ -2014,9 +1954,7 @@
       <c r="P34" s="14"/>
     </row>
     <row r="35" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A35" s="11">
-        <v>31</v>
-      </c>
+      <c r="A35" s="11"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="13"/>
@@ -2034,9 +1972,7 @@
       <c r="P35" s="14"/>
     </row>
     <row r="36" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A36" s="11">
-        <v>32</v>
-      </c>
+      <c r="A36" s="11"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
@@ -2054,9 +1990,7 @@
       <c r="P36" s="14"/>
     </row>
     <row r="37" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A37" s="11">
-        <v>33</v>
-      </c>
+      <c r="A37" s="11"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
@@ -2074,9 +2008,7 @@
       <c r="P37" s="14"/>
     </row>
     <row r="38" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A38" s="11">
-        <v>34</v>
-      </c>
+      <c r="A38" s="11"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="13"/>
@@ -2094,9 +2026,7 @@
       <c r="P38" s="14"/>
     </row>
     <row r="39" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A39" s="11">
-        <v>35</v>
-      </c>
+      <c r="A39" s="11"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="13"/>
@@ -2114,9 +2044,7 @@
       <c r="P39" s="14"/>
     </row>
     <row r="40" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A40" s="11">
-        <v>36</v>
-      </c>
+      <c r="A40" s="11"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
@@ -2134,9 +2062,7 @@
       <c r="P40" s="14"/>
     </row>
     <row r="41" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A41" s="11">
-        <v>37</v>
-      </c>
+      <c r="A41" s="11"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
@@ -2154,9 +2080,7 @@
       <c r="P41" s="14"/>
     </row>
     <row r="42" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A42" s="11">
-        <v>38</v>
-      </c>
+      <c r="A42" s="11"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="13"/>
@@ -2174,9 +2098,7 @@
       <c r="P42" s="14"/>
     </row>
     <row r="43" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A43" s="11">
-        <v>39</v>
-      </c>
+      <c r="A43" s="11"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="13"/>
@@ -2194,9 +2116,7 @@
       <c r="P43" s="14"/>
     </row>
     <row r="44" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A44" s="11">
-        <v>40</v>
-      </c>
+      <c r="A44" s="11"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="13"/>
@@ -2214,9 +2134,7 @@
       <c r="P44" s="14"/>
     </row>
     <row r="45" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A45" s="11">
-        <v>41</v>
-      </c>
+      <c r="A45" s="11"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="13"/>
@@ -2234,9 +2152,7 @@
       <c r="P45" s="14"/>
     </row>
     <row r="46" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A46" s="11">
-        <v>42</v>
-      </c>
+      <c r="A46" s="11"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="13"/>
@@ -2254,9 +2170,7 @@
       <c r="P46" s="14"/>
     </row>
     <row r="47" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A47" s="11">
-        <v>43</v>
-      </c>
+      <c r="A47" s="11"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="13"/>
@@ -2274,9 +2188,7 @@
       <c r="P47" s="14"/>
     </row>
     <row r="48" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A48" s="11">
-        <v>44</v>
-      </c>
+      <c r="A48" s="11"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
@@ -2294,9 +2206,7 @@
       <c r="P48" s="14"/>
     </row>
     <row r="49" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A49" s="11">
-        <v>45</v>
-      </c>
+      <c r="A49" s="11"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
@@ -2314,9 +2224,7 @@
       <c r="P49" s="14"/>
     </row>
     <row r="50" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A50" s="11">
-        <v>46</v>
-      </c>
+      <c r="A50" s="11"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
@@ -2334,9 +2242,7 @@
       <c r="P50" s="14"/>
     </row>
     <row r="51" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A51" s="11">
-        <v>47</v>
-      </c>
+      <c r="A51" s="11"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="13"/>
@@ -2354,9 +2260,7 @@
       <c r="P51" s="14"/>
     </row>
     <row r="52" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A52" s="11">
-        <v>48</v>
-      </c>
+      <c r="A52" s="11"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13"/>
@@ -2374,9 +2278,7 @@
       <c r="P52" s="14"/>
     </row>
     <row r="53" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A53" s="11">
-        <v>49</v>
-      </c>
+      <c r="A53" s="11"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
@@ -2394,9 +2296,7 @@
       <c r="P53" s="14"/>
     </row>
     <row r="54" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A54" s="11">
-        <v>50</v>
-      </c>
+      <c r="A54" s="11"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="13"/>
@@ -2414,9 +2314,7 @@
       <c r="P54" s="14"/>
     </row>
     <row r="55" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A55" s="11">
-        <v>51</v>
-      </c>
+      <c r="A55" s="11"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="13"/>
@@ -2434,9 +2332,7 @@
       <c r="P55" s="14"/>
     </row>
     <row r="56" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A56" s="11">
-        <v>52</v>
-      </c>
+      <c r="A56" s="11"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="13"/>
@@ -2454,9 +2350,7 @@
       <c r="P56" s="14"/>
     </row>
     <row r="57" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A57" s="11">
-        <v>53</v>
-      </c>
+      <c r="A57" s="11"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="13"/>
@@ -2474,9 +2368,7 @@
       <c r="P57" s="14"/>
     </row>
     <row r="58" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A58" s="11">
-        <v>54</v>
-      </c>
+      <c r="A58" s="11"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="13"/>
@@ -2494,9 +2386,7 @@
       <c r="P58" s="14"/>
     </row>
     <row r="59" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A59" s="11">
-        <v>55</v>
-      </c>
+      <c r="A59" s="11"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="13"/>
@@ -2514,9 +2404,7 @@
       <c r="P59" s="14"/>
     </row>
     <row r="60" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A60" s="11">
-        <v>56</v>
-      </c>
+      <c r="A60" s="11"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="13"/>
@@ -2534,9 +2422,7 @@
       <c r="P60" s="14"/>
     </row>
     <row r="61" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A61" s="11">
-        <v>57</v>
-      </c>
+      <c r="A61" s="11"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
@@ -2554,9 +2440,7 @@
       <c r="P61" s="14"/>
     </row>
     <row r="62" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A62" s="11">
-        <v>58</v>
-      </c>
+      <c r="A62" s="11"/>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
@@ -2574,9 +2458,7 @@
       <c r="P62" s="14"/>
     </row>
     <row r="63" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A63" s="11">
-        <v>59</v>
-      </c>
+      <c r="A63" s="11"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
@@ -2594,9 +2476,7 @@
       <c r="P63" s="14"/>
     </row>
     <row r="64" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A64" s="11">
-        <v>60</v>
-      </c>
+      <c r="A64" s="11"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
@@ -2614,9 +2494,7 @@
       <c r="P64" s="14"/>
     </row>
     <row r="65" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A65" s="11">
-        <v>61</v>
-      </c>
+      <c r="A65" s="11"/>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
@@ -2634,9 +2512,7 @@
       <c r="P65" s="14"/>
     </row>
     <row r="66" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A66" s="11">
-        <v>62</v>
-      </c>
+      <c r="A66" s="11"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
@@ -2654,9 +2530,7 @@
       <c r="P66" s="14"/>
     </row>
     <row r="67" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A67" s="11">
-        <v>63</v>
-      </c>
+      <c r="A67" s="11"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -2674,9 +2548,7 @@
       <c r="P67" s="14"/>
     </row>
     <row r="68" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A68" s="11">
-        <v>64</v>
-      </c>
+      <c r="A68" s="11"/>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
@@ -2694,9 +2566,7 @@
       <c r="P68" s="14"/>
     </row>
     <row r="69" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A69" s="11">
-        <v>65</v>
-      </c>
+      <c r="A69" s="11"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
@@ -2714,9 +2584,7 @@
       <c r="P69" s="14"/>
     </row>
     <row r="70" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A70" s="11">
-        <v>66</v>
-      </c>
+      <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
@@ -2734,9 +2602,7 @@
       <c r="P70" s="14"/>
     </row>
     <row r="71" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A71" s="11">
-        <v>67</v>
-      </c>
+      <c r="A71" s="11"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
@@ -2754,9 +2620,7 @@
       <c r="P71" s="14"/>
     </row>
     <row r="72" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A72" s="11">
-        <v>68</v>
-      </c>
+      <c r="A72" s="11"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
@@ -2774,9 +2638,7 @@
       <c r="P72" s="14"/>
     </row>
     <row r="73" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A73" s="11">
-        <v>69</v>
-      </c>
+      <c r="A73" s="11"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
@@ -2794,9 +2656,7 @@
       <c r="P73" s="14"/>
     </row>
     <row r="74" spans="1:16" s="5" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A74" s="15">
-        <v>70</v>
-      </c>
+      <c r="A74" s="15"/>
       <c r="B74" s="16"/>
       <c r="C74" s="16"/>
       <c r="D74" s="17"/>

</xml_diff>